<commit_message>
version debug Objet + attribut / pas de date en str ==> bug
</commit_message>
<xml_diff>
--- a/Classeur1.xlsx
+++ b/Classeur1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gabri\PycharmProjects\POO_ecole_absence\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D25A855-7228-46B4-8C01-58EC6CE7A5D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D40276C1-C914-4581-97D6-BCF4D4FF3ACD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="11424" yWindow="0" windowWidth="11712" windowHeight="12336" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t xml:space="preserve">Nom </t>
   </si>
@@ -54,19 +54,36 @@
   </si>
   <si>
     <t xml:space="preserve">Gabriel </t>
+  </si>
+  <si>
+    <t>damien</t>
+  </si>
+  <si>
+    <t>roger</t>
+  </si>
+  <si>
+    <t>rock</t>
+  </si>
+  <si>
+    <t>basile</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="JetBrains Mono"/>
+      <family val="3"/>
     </font>
   </fonts>
   <fills count="2">
@@ -89,9 +106,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -406,18 +426,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:C65536"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
   <cols>
     <col min="3" max="3" width="22.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -428,7 +448,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -439,7 +459,7 @@
         <v>44966</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -450,7 +470,28 @@
         <v>45080</v>
       </c>
     </row>
+    <row r="4" spans="1:3">
+      <c r="B4" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="B5" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="B6" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="B7" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
fin recherche data, reload. debut application
</commit_message>
<xml_diff>
--- a/Classeur1.xlsx
+++ b/Classeur1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gabri\PycharmProjects\POO_ecole_absence\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD364274-2FC1-4A68-A088-B9A29E09CCF2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A23E9A7-6FDA-486E-AFDB-F135147B5A23}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="22932" yWindow="1032" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t xml:space="preserve">Nom </t>
   </si>
@@ -63,9 +63,6 @@
   </si>
   <si>
     <t xml:space="preserve">gerard </t>
-  </si>
-  <si>
-    <t xml:space="preserve">rober </t>
   </si>
 </sst>
 </file>
@@ -482,9 +479,6 @@
       </c>
     </row>
     <row r="5" spans="1:3">
-      <c r="A5" t="s">
-        <v>10</v>
-      </c>
       <c r="B5" s="2" t="s">
         <v>9</v>
       </c>

</xml_diff>